<commit_message>
MetricSheet first pass done.  Starting FaeSheet.
</commit_message>
<xml_diff>
--- a/Queries/Queries/test.xlsx
+++ b/Queries/Queries/test.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="69">
   <si>
     <t>Activity</t>
   </si>
@@ -162,6 +162,66 @@
   </si>
   <si>
     <t>Customer 'Other'</t>
+  </si>
+  <si>
+    <t>Support Agreement (Software) - 10</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>Finland</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Other (EMEA)</t>
+  </si>
+  <si>
+    <t>Support Agreement (Hardware) - 11</t>
+  </si>
+  <si>
+    <t>Pre Sales Support - 12</t>
+  </si>
+  <si>
+    <t>Post Sales support (Non contract) - 13</t>
+  </si>
+  <si>
+    <t>Post Sales support (SW-Customer Funded) - 14</t>
+  </si>
+  <si>
+    <t>Post Sales support (HW-Customer Funded) - 15</t>
+  </si>
+  <si>
+    <t>NRE (Customer funded) - 16</t>
+  </si>
+  <si>
+    <t>Training - Providing - Non Customer Specific - 17</t>
+  </si>
+  <si>
+    <t>Training - Providing - Customer Specific - 18</t>
+  </si>
+  <si>
+    <t>Training - Receiving - Non Customer Specific - 19</t>
+  </si>
+  <si>
+    <t>Training - Receiving - Customer Specific - 20</t>
+  </si>
+  <si>
+    <t>Internal Business Meeting - 21</t>
+  </si>
+  <si>
+    <t>Professional Services - 22</t>
+  </si>
+  <si>
+    <t>Post Sales Support (Warranty Period) - 23</t>
   </si>
 </sst>
 </file>
@@ -639,7 +699,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:P55"/>
+  <dimension ref="B2:P167"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2161,6 +2221,9 @@
         <v>12</v>
       </c>
       <c r="O38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P38" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2204,8 +2267,11 @@
       <c r="N39" s="3" t="n">
         <v>152</v>
       </c>
-      <c r="O39" s="4" t="n">
-        <v>69.29166666666667</v>
+      <c r="O39" s="3" t="n">
+        <v>138</v>
+      </c>
+      <c r="P39" s="4" t="n">
+        <v>63.96153846153846</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="40" spans="1:16">
@@ -2248,8 +2314,11 @@
       <c r="N40" s="3" t="n">
         <v>733</v>
       </c>
-      <c r="O40" s="4" t="n">
-        <v>717.9583333333334</v>
+      <c r="O40" s="3" t="n">
+        <v>701</v>
+      </c>
+      <c r="P40" s="4" t="n">
+        <v>662.7307692307693</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="41" spans="1:16">
@@ -2292,8 +2361,11 @@
       <c r="N41" s="5" t="n">
         <v>20.73669849931787</v>
       </c>
-      <c r="O41" s="6" t="n">
-        <v>9.783388688369994</v>
+      <c r="O41" s="5" t="n">
+        <v>19.68616262482168</v>
+      </c>
+      <c r="P41" s="6" t="n">
+        <v>9.030820327726149</v>
       </c>
     </row>
     <row customHeight="1" ht="40" r="43" spans="1:16">
@@ -2724,46 +2796,46 @@
         <v>46</v>
       </c>
       <c r="C53" s="3" t="n">
-        <v>59</v>
+        <v>17</v>
       </c>
       <c r="D53" s="3" t="n">
-        <v>63</v>
+        <v>22</v>
       </c>
       <c r="E53" s="3" t="n">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="F53" s="3" t="n">
-        <v>10</v>
+        <v>22.5</v>
       </c>
       <c r="G53" s="3" t="n">
-        <v>13</v>
+        <v>37.5</v>
       </c>
       <c r="H53" s="3" t="n">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="I53" s="3" t="n">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="J53" s="3" t="n">
-        <v>39</v>
+        <v>83</v>
       </c>
       <c r="K53" s="3" t="n">
-        <v>223.5</v>
+        <v>18</v>
       </c>
       <c r="L53" s="3" t="n">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="M53" s="3" t="n">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="N53" s="3" t="n">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="O53" s="3" t="n">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="P53" s="4" t="n">
-        <v>50.96153846153846</v>
+        <v>29.53846153846154</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="54" spans="1:16">
@@ -2771,46 +2843,46 @@
         <v>47</v>
       </c>
       <c r="C54" s="3" t="n">
+        <v>59</v>
+      </c>
+      <c r="D54" s="3" t="n">
+        <v>63</v>
+      </c>
+      <c r="E54" s="3" t="n">
         <v>17</v>
       </c>
-      <c r="D54" s="3" t="n">
-        <v>22</v>
-      </c>
-      <c r="E54" s="3" t="n">
-        <v>28</v>
-      </c>
       <c r="F54" s="3" t="n">
-        <v>22.5</v>
+        <v>10</v>
       </c>
       <c r="G54" s="3" t="n">
-        <v>37.5</v>
+        <v>13</v>
       </c>
       <c r="H54" s="3" t="n">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="I54" s="3" t="n">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="J54" s="3" t="n">
-        <v>83</v>
+        <v>39</v>
       </c>
       <c r="K54" s="3" t="n">
-        <v>18</v>
+        <v>223.5</v>
       </c>
       <c r="L54" s="3" t="n">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="M54" s="3" t="n">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="N54" s="3" t="n">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="O54" s="3" t="n">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="P54" s="4" t="n">
-        <v>29.53846153846154</v>
+        <v>50.96153846153846</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="55" spans="1:16">
@@ -2858,6 +2930,4612 @@
       </c>
       <c r="P55" s="6" t="n">
         <v>9.076923076923077</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="40" r="57" spans="1:16">
+      <c r="B57" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L57" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M57" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N57" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O57" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P57" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="58" spans="1:16">
+      <c r="B58" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C58" s="3" t="n">
+        <v>68.5</v>
+      </c>
+      <c r="D58" s="3" t="n">
+        <v>93.5</v>
+      </c>
+      <c r="E58" s="3" t="n">
+        <v>46</v>
+      </c>
+      <c r="F58" s="3" t="n">
+        <v>28.5</v>
+      </c>
+      <c r="G58" s="3" t="n">
+        <v>96.5</v>
+      </c>
+      <c r="H58" s="3" t="n">
+        <v>48.5</v>
+      </c>
+      <c r="I58" s="3" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="J58" s="3" t="n">
+        <v>64</v>
+      </c>
+      <c r="K58" s="3" t="n">
+        <v>35</v>
+      </c>
+      <c r="L58" s="3" t="n">
+        <v>56</v>
+      </c>
+      <c r="M58" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="N58" s="3" t="n">
+        <v>58</v>
+      </c>
+      <c r="O58" s="3" t="n">
+        <v>47</v>
+      </c>
+      <c r="P58" s="4" t="n">
+        <v>51.07692307692308</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="59" spans="1:16">
+      <c r="B59" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C59" s="3" t="n">
+        <v>130.5</v>
+      </c>
+      <c r="D59" s="3" t="n">
+        <v>176.5</v>
+      </c>
+      <c r="E59" s="3" t="n">
+        <v>161</v>
+      </c>
+      <c r="F59" s="3" t="n">
+        <v>157.5</v>
+      </c>
+      <c r="G59" s="3" t="n">
+        <v>117</v>
+      </c>
+      <c r="H59" s="3" t="n">
+        <v>143</v>
+      </c>
+      <c r="I59" s="3" t="n">
+        <v>190.5</v>
+      </c>
+      <c r="J59" s="3" t="n">
+        <v>145.5</v>
+      </c>
+      <c r="K59" s="3" t="n">
+        <v>174</v>
+      </c>
+      <c r="L59" s="3" t="n">
+        <v>157</v>
+      </c>
+      <c r="M59" s="3" t="n">
+        <v>155</v>
+      </c>
+      <c r="N59" s="3" t="n">
+        <v>124</v>
+      </c>
+      <c r="O59" s="3" t="n">
+        <v>98</v>
+      </c>
+      <c r="P59" s="4" t="n">
+        <v>148.4230769230769</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="60" spans="1:16">
+      <c r="B60" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C60" s="3" t="n">
+        <v>98</v>
+      </c>
+      <c r="D60" s="3" t="n">
+        <v>75.5</v>
+      </c>
+      <c r="E60" s="3" t="n">
+        <v>142</v>
+      </c>
+      <c r="F60" s="3" t="n">
+        <v>140.5</v>
+      </c>
+      <c r="G60" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="H60" s="3" t="n">
+        <v>154.5</v>
+      </c>
+      <c r="I60" s="3" t="n">
+        <v>205</v>
+      </c>
+      <c r="J60" s="3" t="n">
+        <v>167.5</v>
+      </c>
+      <c r="K60" s="3" t="n">
+        <v>106.5</v>
+      </c>
+      <c r="L60" s="3" t="n">
+        <v>87</v>
+      </c>
+      <c r="M60" s="3" t="n">
+        <v>144</v>
+      </c>
+      <c r="N60" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="O60" s="3" t="n">
+        <v>56</v>
+      </c>
+      <c r="P60" s="4" t="n">
+        <v>116.6538461538462</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="61" spans="1:16">
+      <c r="B61" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D61" s="3" t="n">
+        <v>76</v>
+      </c>
+      <c r="E61" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="F61" s="3" t="n">
+        <v>76</v>
+      </c>
+      <c r="G61" s="3" t="n">
+        <v>68</v>
+      </c>
+      <c r="H61" s="3" t="n">
+        <v>60</v>
+      </c>
+      <c r="I61" s="3" t="n">
+        <v>56</v>
+      </c>
+      <c r="J61" s="3" t="n">
+        <v>48</v>
+      </c>
+      <c r="K61" s="3" t="n">
+        <v>80</v>
+      </c>
+      <c r="L61" s="3" t="n">
+        <v>68</v>
+      </c>
+      <c r="M61" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="N61" s="3" t="n">
+        <v>64</v>
+      </c>
+      <c r="O61" s="3" t="n">
+        <v>48</v>
+      </c>
+      <c r="P61" s="4" t="n">
+        <v>55.69230769230769</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="62" spans="1:16">
+      <c r="B62" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C62" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D62" s="3" t="n">
+        <v>28.5</v>
+      </c>
+      <c r="E62" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="F62" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G62" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="H62" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="I62" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J62" s="3" t="n">
+        <v>19.5</v>
+      </c>
+      <c r="K62" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L62" s="3" t="n">
+        <v>18.5</v>
+      </c>
+      <c r="M62" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="N62" s="3" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="O62" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="P62" s="4" t="n">
+        <v>11.38461538461539</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="63" spans="1:16">
+      <c r="B63" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C63" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D63" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E63" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F63" s="5" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="G63" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H63" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I63" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J63" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="K63" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L63" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M63" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="N63" s="5" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="O63" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="P63" s="6" t="n">
+        <v>2.769230769230769</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="40" r="65" spans="1:16">
+      <c r="B65" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L65" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M65" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N65" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O65" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P65" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="66" spans="1:16">
+      <c r="B66" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C66" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D66" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E66" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="F66" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G66" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H66" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="I66" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J66" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K66" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L66" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="M66" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N66" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O66" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P66" s="4" t="n">
+        <v>1.615384615384615</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="67" spans="1:16">
+      <c r="B67" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C67" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="D67" s="3" t="n">
+        <v>21.5</v>
+      </c>
+      <c r="E67" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="F67" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="G67" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="H67" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="I67" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="J67" s="3" t="n">
+        <v>26.5</v>
+      </c>
+      <c r="K67" s="3" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="L67" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M67" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="N67" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="O67" s="3" t="n">
+        <v>29.5</v>
+      </c>
+      <c r="P67" s="4" t="n">
+        <v>17.69230769230769</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="68" spans="1:16">
+      <c r="B68" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C68" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D68" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="E68" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="F68" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="G68" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="H68" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I68" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J68" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K68" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L68" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M68" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N68" s="3" t="n">
+        <v>50.5</v>
+      </c>
+      <c r="O68" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="P68" s="4" t="n">
+        <v>7.961538461538462</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="69" spans="1:16">
+      <c r="B69" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C69" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D69" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E69" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F69" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G69" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="H69" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I69" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J69" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K69" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L69" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M69" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N69" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O69" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P69" s="4" t="n">
+        <v>0.3076923076923077</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="70" spans="1:16">
+      <c r="B70" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C70" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D70" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E70" s="3" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="F70" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G70" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H70" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I70" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J70" s="3" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="K70" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L70" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="M70" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N70" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O70" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P70" s="4" t="n">
+        <v>2.538461538461538</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="71" spans="1:16">
+      <c r="B71" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C71" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D71" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E71" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F71" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G71" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H71" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I71" s="5" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="J71" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K71" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L71" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M71" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N71" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O71" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P71" s="6" t="n">
+        <v>0.4230769230769231</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="40" r="73" spans="1:16">
+      <c r="B73" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I73" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J73" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K73" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L73" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M73" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N73" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O73" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P73" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="74" spans="1:16">
+      <c r="B74" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C74" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D74" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E74" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F74" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G74" s="3" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="H74" s="3" t="n">
+        <v>18.5</v>
+      </c>
+      <c r="I74" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="J74" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K74" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L74" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="M74" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="N74" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="O74" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="P74" s="4" t="n">
+        <v>6.846153846153846</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="75" spans="1:16">
+      <c r="B75" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C75" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D75" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="E75" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="F75" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="G75" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="H75" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="I75" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="J75" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="K75" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="L75" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="M75" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="N75" s="3" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="O75" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="P75" s="4" t="n">
+        <v>8.961538461538462</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="76" spans="1:16">
+      <c r="B76" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C76" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D76" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E76" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F76" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G76" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H76" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="I76" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="J76" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K76" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L76" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M76" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N76" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O76" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P76" s="4" t="n">
+        <v>1.230769230769231</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="77" spans="1:16">
+      <c r="B77" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C77" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D77" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E77" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F77" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G77" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H77" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I77" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J77" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K77" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L77" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M77" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N77" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="O77" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P77" s="4" t="n">
+        <v>1.230769230769231</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="78" spans="1:16">
+      <c r="B78" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C78" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D78" s="3" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="E78" s="3" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F78" s="3" t="n">
+        <v>46</v>
+      </c>
+      <c r="G78" s="3" t="n">
+        <v>19.5</v>
+      </c>
+      <c r="H78" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I78" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J78" s="3" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="K78" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="L78" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="M78" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N78" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O78" s="3" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="P78" s="4" t="n">
+        <v>7.653846153846154</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="79" spans="1:16">
+      <c r="B79" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C79" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D79" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E79" s="5" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F79" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G79" s="5" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="H79" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="I79" s="5" t="n">
+        <v>86.5</v>
+      </c>
+      <c r="J79" s="5" t="n">
+        <v>71</v>
+      </c>
+      <c r="K79" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="L79" s="5" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="M79" s="5" t="n">
+        <v>95.5</v>
+      </c>
+      <c r="N79" s="5" t="n">
+        <v>20.5</v>
+      </c>
+      <c r="O79" s="5" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="P79" s="6" t="n">
+        <v>24.26923076923077</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="40" r="81" spans="1:16">
+      <c r="B81" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I81" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J81" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K81" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L81" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M81" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N81" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O81" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P81" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="82" spans="1:16">
+      <c r="B82" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C82" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="D82" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="E82" s="3" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="F82" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="G82" s="3" t="n">
+        <v>51</v>
+      </c>
+      <c r="H82" s="3" t="n">
+        <v>44.5</v>
+      </c>
+      <c r="I82" s="3" t="n">
+        <v>39</v>
+      </c>
+      <c r="J82" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="K82" s="3" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="L82" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M82" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="N82" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="O82" s="3" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="P82" s="4" t="n">
+        <v>28.69230769230769</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="83" spans="1:16">
+      <c r="B83" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C83" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D83" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E83" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F83" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G83" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H83" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I83" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J83" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K83" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L83" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M83" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N83" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O83" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P83" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="84" spans="1:16">
+      <c r="B84" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C84" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D84" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E84" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F84" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G84" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H84" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I84" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J84" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K84" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L84" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M84" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N84" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O84" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P84" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="85" spans="1:16">
+      <c r="B85" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C85" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D85" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E85" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F85" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G85" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H85" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I85" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J85" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K85" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L85" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M85" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N85" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O85" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P85" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="86" spans="1:16">
+      <c r="B86" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C86" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D86" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E86" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F86" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G86" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H86" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I86" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J86" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K86" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L86" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M86" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N86" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O86" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P86" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="87" spans="1:16">
+      <c r="B87" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C87" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="D87" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="E87" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F87" s="5" t="n">
+        <v>46.5</v>
+      </c>
+      <c r="G87" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H87" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I87" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J87" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K87" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L87" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M87" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N87" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O87" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P87" s="6" t="n">
+        <v>4.269230769230769</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="40" r="89" spans="1:16">
+      <c r="B89" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I89" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J89" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K89" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L89" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M89" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N89" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O89" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P89" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="90" spans="1:16">
+      <c r="B90" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C90" s="3" t="n">
+        <v>16.5</v>
+      </c>
+      <c r="D90" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E90" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F90" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G90" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H90" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I90" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="J90" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="K90" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L90" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M90" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="N90" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="O90" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P90" s="4" t="n">
+        <v>5.807692307692307</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="91" spans="1:16">
+      <c r="B91" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C91" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D91" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E91" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F91" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G91" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H91" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I91" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J91" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="K91" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="L91" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="M91" s="3" t="n">
+        <v>41.5</v>
+      </c>
+      <c r="N91" s="3" t="n">
+        <v>34.5</v>
+      </c>
+      <c r="O91" s="3" t="n">
+        <v>41.5</v>
+      </c>
+      <c r="P91" s="4" t="n">
+        <v>12.88461538461539</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="92" spans="1:16">
+      <c r="B92" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C92" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D92" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E92" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F92" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G92" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H92" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I92" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J92" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K92" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L92" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M92" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N92" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O92" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P92" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="93" spans="1:16">
+      <c r="B93" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C93" s="3" t="n">
+        <v>32</v>
+      </c>
+      <c r="D93" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E93" s="3" t="n">
+        <v>39</v>
+      </c>
+      <c r="F93" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G93" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H93" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I93" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J93" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K93" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L93" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M93" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N93" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O93" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P93" s="4" t="n">
+        <v>5.461538461538462</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="94" spans="1:16">
+      <c r="B94" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C94" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D94" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E94" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F94" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G94" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H94" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I94" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J94" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K94" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L94" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M94" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N94" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O94" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P94" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="95" spans="1:16">
+      <c r="B95" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C95" s="5" t="n">
+        <v>16.5</v>
+      </c>
+      <c r="D95" s="5" t="n">
+        <v>56</v>
+      </c>
+      <c r="E95" s="5" t="n">
+        <v>52.5</v>
+      </c>
+      <c r="F95" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G95" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H95" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I95" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J95" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K95" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L95" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M95" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N95" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O95" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P95" s="6" t="n">
+        <v>9.615384615384615</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="40" r="97" spans="1:16">
+      <c r="B97" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H97" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I97" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J97" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K97" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L97" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M97" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N97" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O97" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P97" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="98" spans="1:16">
+      <c r="B98" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C98" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D98" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E98" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F98" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G98" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="H98" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I98" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J98" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K98" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L98" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M98" s="3" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="N98" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="O98" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P98" s="4" t="n">
+        <v>1.653846153846154</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="99" spans="1:16">
+      <c r="B99" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C99" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D99" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E99" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F99" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G99" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H99" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I99" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J99" s="3" t="n">
+        <v>24.5</v>
+      </c>
+      <c r="K99" s="3" t="n">
+        <v>24.5</v>
+      </c>
+      <c r="L99" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="M99" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N99" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O99" s="3" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="P99" s="4" t="n">
+        <v>5.807692307692307</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="100" spans="1:16">
+      <c r="B100" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C100" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D100" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E100" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F100" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G100" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H100" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I100" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J100" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K100" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L100" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M100" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N100" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O100" s="3" t="n">
+        <v>43.5</v>
+      </c>
+      <c r="P100" s="4" t="n">
+        <v>3.346153846153846</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="101" spans="1:16">
+      <c r="B101" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C101" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D101" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E101" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F101" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G101" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H101" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I101" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J101" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K101" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L101" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M101" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N101" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O101" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P101" s="4" t="n">
+        <v>0.6153846153846154</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="102" spans="1:16">
+      <c r="B102" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C102" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D102" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E102" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F102" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G102" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H102" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I102" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J102" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K102" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L102" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M102" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N102" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O102" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P102" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="103" spans="1:16">
+      <c r="B103" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C103" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D103" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E103" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F103" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G103" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H103" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I103" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J103" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K103" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L103" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M103" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N103" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O103" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P103" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="40" r="105" spans="1:16">
+      <c r="B105" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G105" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H105" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I105" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J105" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K105" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L105" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M105" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N105" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O105" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P105" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="106" spans="1:16">
+      <c r="B106" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C106" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D106" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E106" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F106" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G106" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H106" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I106" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J106" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K106" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L106" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M106" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N106" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O106" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P106" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="107" spans="1:16">
+      <c r="B107" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C107" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D107" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E107" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F107" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G107" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H107" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I107" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J107" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K107" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L107" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M107" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N107" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O107" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P107" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="108" spans="1:16">
+      <c r="B108" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C108" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D108" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E108" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F108" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G108" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H108" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I108" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J108" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K108" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L108" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M108" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N108" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O108" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P108" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="109" spans="1:16">
+      <c r="B109" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C109" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D109" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E109" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F109" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G109" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H109" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I109" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J109" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K109" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L109" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M109" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N109" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O109" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P109" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="110" spans="1:16">
+      <c r="B110" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C110" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D110" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E110" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F110" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G110" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H110" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I110" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J110" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K110" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L110" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M110" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N110" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O110" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P110" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="111" spans="1:16">
+      <c r="B111" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C111" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D111" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E111" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F111" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G111" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H111" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I111" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J111" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K111" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L111" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M111" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N111" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O111" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P111" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="40" r="113" spans="1:16">
+      <c r="B113" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G113" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H113" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I113" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J113" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K113" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L113" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M113" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N113" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O113" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P113" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="114" spans="1:16">
+      <c r="B114" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C114" s="3" t="n">
+        <v>39.5</v>
+      </c>
+      <c r="D114" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="E114" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="F114" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G114" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="H114" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="I114" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="J114" s="3" t="n">
+        <v>41</v>
+      </c>
+      <c r="K114" s="3" t="n">
+        <v>76</v>
+      </c>
+      <c r="L114" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="M114" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="N114" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="O114" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="P114" s="4" t="n">
+        <v>27.5</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="115" spans="1:16">
+      <c r="B115" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C115" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D115" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E115" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F115" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G115" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H115" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I115" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J115" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K115" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L115" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M115" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N115" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O115" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P115" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="116" spans="1:16">
+      <c r="B116" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C116" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D116" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E116" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F116" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="G116" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H116" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I116" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J116" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K116" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L116" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M116" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N116" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O116" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P116" s="4" t="n">
+        <v>0.5384615384615384</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="117" spans="1:16">
+      <c r="B117" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C117" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D117" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E117" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F117" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G117" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H117" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I117" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J117" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K117" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L117" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="M117" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="N117" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O117" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P117" s="4" t="n">
+        <v>1.230769230769231</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="118" spans="1:16">
+      <c r="B118" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C118" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D118" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E118" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F118" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G118" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H118" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I118" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J118" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K118" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L118" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M118" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N118" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O118" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P118" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="119" spans="1:16">
+      <c r="B119" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C119" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D119" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E119" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F119" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G119" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H119" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I119" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J119" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K119" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L119" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M119" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N119" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O119" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P119" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="40" r="121" spans="1:16">
+      <c r="B121" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G121" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H121" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I121" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J121" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K121" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L121" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M121" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N121" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O121" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P121" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="122" spans="1:16">
+      <c r="B122" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C122" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D122" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E122" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F122" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G122" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H122" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I122" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J122" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K122" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="L122" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="M122" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N122" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O122" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P122" s="4" t="n">
+        <v>1.153846153846154</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="123" spans="1:16">
+      <c r="B123" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C123" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D123" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E123" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F123" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G123" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H123" s="3" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="I123" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J123" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K123" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L123" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="M123" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="N123" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="O123" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="P123" s="4" t="n">
+        <v>3.653846153846154</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="124" spans="1:16">
+      <c r="B124" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C124" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D124" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E124" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F124" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G124" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H124" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I124" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J124" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K124" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L124" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M124" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N124" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O124" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P124" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="125" spans="1:16">
+      <c r="B125" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C125" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D125" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E125" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F125" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G125" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H125" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I125" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J125" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K125" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L125" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="M125" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N125" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O125" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P125" s="4" t="n">
+        <v>0.3076923076923077</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="126" spans="1:16">
+      <c r="B126" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C126" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D126" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E126" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F126" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G126" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H126" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I126" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J126" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K126" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L126" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M126" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N126" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O126" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P126" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="127" spans="1:16">
+      <c r="B127" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C127" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D127" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E127" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F127" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G127" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H127" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I127" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J127" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K127" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L127" s="5" t="n">
+        <v>52</v>
+      </c>
+      <c r="M127" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N127" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O127" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P127" s="6" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="40" r="129" spans="1:16">
+      <c r="B129" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F129" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G129" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H129" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I129" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J129" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K129" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L129" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M129" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N129" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O129" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P129" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="130" spans="1:16">
+      <c r="B130" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C130" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="D130" s="3" t="n">
+        <v>54</v>
+      </c>
+      <c r="E130" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F130" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="G130" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H130" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I130" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J130" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="K130" s="3" t="n">
+        <v>105.5</v>
+      </c>
+      <c r="L130" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="M130" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="N130" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="O130" s="3" t="n">
+        <v>54</v>
+      </c>
+      <c r="P130" s="4" t="n">
+        <v>20.57692307692308</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="131" spans="1:16">
+      <c r="B131" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C131" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D131" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E131" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F131" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G131" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H131" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I131" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J131" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K131" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="L131" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M131" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N131" s="3" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="O131" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P131" s="4" t="n">
+        <v>1.269230769230769</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="132" spans="1:16">
+      <c r="B132" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C132" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D132" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E132" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F132" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G132" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H132" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I132" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J132" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K132" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L132" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M132" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N132" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O132" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P132" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="133" spans="1:16">
+      <c r="B133" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C133" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D133" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E133" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F133" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G133" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H133" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I133" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J133" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K133" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L133" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M133" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N133" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O133" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P133" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="134" spans="1:16">
+      <c r="B134" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C134" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D134" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E134" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F134" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G134" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H134" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I134" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J134" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K134" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L134" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M134" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N134" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O134" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P134" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="135" spans="1:16">
+      <c r="B135" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C135" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D135" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E135" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F135" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G135" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H135" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I135" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J135" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K135" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L135" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M135" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N135" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O135" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P135" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="40" r="137" spans="1:16">
+      <c r="B137" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G137" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H137" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I137" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J137" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K137" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L137" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M137" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N137" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O137" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P137" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="138" spans="1:16">
+      <c r="B138" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C138" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D138" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E138" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F138" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G138" s="3" t="n">
+        <v>42</v>
+      </c>
+      <c r="H138" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="I138" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J138" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K138" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L138" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M138" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N138" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O138" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P138" s="4" t="n">
+        <v>3.384615384615385</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="139" spans="1:16">
+      <c r="B139" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C139" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D139" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E139" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F139" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G139" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H139" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I139" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J139" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K139" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L139" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M139" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N139" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O139" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P139" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="140" spans="1:16">
+      <c r="B140" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C140" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D140" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E140" s="3" t="n">
+        <v>35.5</v>
+      </c>
+      <c r="F140" s="3" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="G140" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H140" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I140" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J140" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K140" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L140" s="3" t="n">
+        <v>38</v>
+      </c>
+      <c r="M140" s="3" t="n">
+        <v>36</v>
+      </c>
+      <c r="N140" s="3" t="n">
+        <v>17.5</v>
+      </c>
+      <c r="O140" s="3" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="P140" s="4" t="n">
+        <v>10.61538461538461</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="141" spans="1:16">
+      <c r="B141" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C141" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D141" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E141" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F141" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G141" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H141" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I141" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J141" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K141" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L141" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="M141" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N141" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O141" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P141" s="4" t="n">
+        <v>0.6153846153846154</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="142" spans="1:16">
+      <c r="B142" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C142" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D142" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E142" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F142" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G142" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H142" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I142" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J142" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K142" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L142" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M142" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N142" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O142" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P142" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="143" spans="1:16">
+      <c r="B143" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C143" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D143" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E143" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F143" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G143" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H143" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I143" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J143" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K143" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L143" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M143" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N143" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O143" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P143" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="40" r="145" spans="1:16">
+      <c r="B145" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F145" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G145" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H145" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I145" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J145" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K145" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L145" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M145" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N145" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O145" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P145" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="146" spans="1:16">
+      <c r="B146" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C146" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D146" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E146" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F146" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G146" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H146" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="I146" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="J146" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K146" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L146" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M146" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N146" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O146" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P146" s="4" t="n">
+        <v>1.076923076923077</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="147" spans="1:16">
+      <c r="B147" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C147" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D147" s="3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E147" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F147" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G147" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H147" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I147" s="3" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="J147" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K147" s="3" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="L147" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M147" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="N147" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O147" s="3" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="P147" s="4" t="n">
+        <v>1.615384615384615</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="148" spans="1:16">
+      <c r="B148" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C148" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D148" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E148" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F148" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G148" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="H148" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I148" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J148" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K148" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L148" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M148" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N148" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O148" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P148" s="4" t="n">
+        <v>1.153846153846154</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="149" spans="1:16">
+      <c r="B149" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C149" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D149" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E149" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F149" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G149" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H149" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I149" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J149" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K149" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L149" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M149" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N149" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O149" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P149" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="150" spans="1:16">
+      <c r="B150" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C150" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D150" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E150" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F150" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G150" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H150" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I150" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J150" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K150" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L150" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M150" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N150" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O150" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P150" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="151" spans="1:16">
+      <c r="B151" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C151" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D151" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E151" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F151" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G151" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H151" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I151" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J151" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K151" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L151" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M151" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N151" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O151" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P151" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="40" r="153" spans="1:16">
+      <c r="B153" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E153" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F153" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G153" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H153" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I153" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J153" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K153" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L153" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M153" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N153" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O153" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P153" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="154" spans="1:16">
+      <c r="B154" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C154" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D154" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E154" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F154" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G154" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H154" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I154" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J154" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K154" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L154" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="M154" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N154" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O154" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P154" s="4" t="n">
+        <v>0.2307692307692308</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="155" spans="1:16">
+      <c r="B155" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C155" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D155" s="3" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="E155" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="F155" s="3" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="G155" s="3" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H155" s="3" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="I155" s="3" t="n">
+        <v>42</v>
+      </c>
+      <c r="J155" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="K155" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L155" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M155" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N155" s="3" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="O155" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P155" s="4" t="n">
+        <v>10.65384615384615</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="156" spans="1:16">
+      <c r="B156" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C156" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D156" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E156" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F156" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G156" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H156" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I156" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J156" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K156" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L156" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M156" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N156" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O156" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P156" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="157" spans="1:16">
+      <c r="B157" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C157" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D157" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E157" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F157" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G157" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H157" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I157" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J157" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K157" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L157" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M157" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N157" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O157" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P157" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="158" spans="1:16">
+      <c r="B158" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C158" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D158" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E158" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F158" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G158" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H158" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I158" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J158" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K158" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L158" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M158" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N158" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O158" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P158" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="159" spans="1:16">
+      <c r="B159" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C159" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D159" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E159" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F159" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G159" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H159" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I159" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J159" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K159" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L159" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M159" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N159" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O159" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P159" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="40" r="161" spans="1:16">
+      <c r="B161" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D161" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E161" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F161" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G161" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H161" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I161" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J161" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K161" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L161" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M161" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N161" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O161" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P161" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="162" spans="1:16">
+      <c r="B162" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C162" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D162" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E162" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F162" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G162" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H162" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I162" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="J162" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K162" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L162" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="M162" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N162" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O162" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P162" s="4" t="n">
+        <v>0.3846153846153846</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="163" spans="1:16">
+      <c r="B163" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C163" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D163" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E163" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F163" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G163" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H163" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I163" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J163" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K163" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L163" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M163" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N163" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O163" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P163" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="164" spans="1:16">
+      <c r="B164" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C164" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D164" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E164" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F164" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G164" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H164" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I164" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J164" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K164" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L164" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M164" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N164" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O164" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P164" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="165" spans="1:16">
+      <c r="B165" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C165" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D165" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E165" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F165" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G165" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H165" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I165" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J165" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K165" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L165" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M165" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N165" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O165" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P165" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="166" spans="1:16">
+      <c r="B166" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C166" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D166" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E166" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F166" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G166" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H166" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I166" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J166" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K166" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L166" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M166" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N166" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O166" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P166" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="167" spans="1:16">
+      <c r="B167" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C167" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D167" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E167" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F167" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G167" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H167" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I167" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J167" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K167" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L167" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M167" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N167" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O167" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P167" s="6" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pretty much done with FAE sheet.
</commit_message>
<xml_diff>
--- a/Queries/Queries/test.xlsx
+++ b/Queries/Queries/test.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
   <si>
     <t>Actual Working Hours</t>
   </si>
@@ -120,6 +120,18 @@
   </si>
   <si>
     <t>Working Hours</t>
+  </si>
+  <si>
+    <t>Internal vs Contract Hours</t>
+  </si>
+  <si>
+    <t>Internal Hours</t>
+  </si>
+  <si>
+    <t>Contractor Hours</t>
+  </si>
+  <si>
+    <t>Additional Hours</t>
   </si>
 </sst>
 </file>
@@ -144,7 +156,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -257,11 +269,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="00000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="00000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="00000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -285,6 +327,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="5" fillId="0" fontId="0" numFmtId="2" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="8" fillId="0" fontId="0" numFmtId="2" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="9" fillId="0" fontId="0" numFmtId="2" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -603,7 +651,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:R38"/>
+  <dimension ref="B2:R61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -694,16 +742,16 @@
         <v>52.5</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>37.5</v>
+        <v>0</v>
       </c>
       <c r="G3" s="3" t="n">
-        <v>37.5</v>
+        <v>0</v>
       </c>
       <c r="H3" s="3" t="n">
-        <v>37.5</v>
+        <v>0</v>
       </c>
       <c r="I3" s="3" t="n">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J3" s="3" t="n">
         <v>59</v>
@@ -715,16 +763,16 @@
         <v>52</v>
       </c>
       <c r="M3" s="3" t="n">
-        <v>38.5</v>
+        <v>35.5</v>
       </c>
       <c r="N3" s="3" t="n">
-        <v>42.5</v>
+        <v>34.5</v>
       </c>
       <c r="O3" s="3" t="n">
         <v>48.5</v>
       </c>
       <c r="P3" s="4" t="n">
-        <v>48.76923076923077</v>
+        <v>39.03846153846154</v>
       </c>
       <c r="Q3" s="3" t="n">
         <v>37.5</v>
@@ -747,7 +795,7 @@
         <v>60.5</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="G4" s="3" t="n">
         <v>40</v>
@@ -762,7 +810,7 @@
         <v>50.5</v>
       </c>
       <c r="K4" s="3" t="n">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L4" s="3" t="n">
         <v>47</v>
@@ -771,13 +819,13 @@
         <v>66</v>
       </c>
       <c r="N4" s="3" t="n">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="O4" s="3" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="P4" s="4" t="n">
-        <v>49.26923076923077</v>
+        <v>46.42307692307692</v>
       </c>
       <c r="Q4" s="3" t="n">
         <v>37.5</v>
@@ -800,7 +848,7 @@
         <v>37.5</v>
       </c>
       <c r="F5" s="3" t="n">
-        <v>37.5</v>
+        <v>15</v>
       </c>
       <c r="G5" s="3" t="n">
         <v>37.5</v>
@@ -824,13 +872,13 @@
         <v>38</v>
       </c>
       <c r="N5" s="3" t="n">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="O5" s="3" t="n">
-        <v>37.5</v>
+        <v>21.5</v>
       </c>
       <c r="P5" s="4" t="n">
-        <v>38</v>
+        <v>34.42307692307692</v>
       </c>
       <c r="Q5" s="3" t="n">
         <v>37.5</v>
@@ -877,13 +925,13 @@
         <v>42</v>
       </c>
       <c r="N6" s="3" t="n">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="O6" s="3" t="n">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="P6" s="4" t="n">
-        <v>44.80769230769231</v>
+        <v>43.57692307692308</v>
       </c>
       <c r="Q6" s="3" t="n">
         <v>37.5</v>
@@ -930,13 +978,13 @@
         <v>42</v>
       </c>
       <c r="N7" s="3" t="n">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="O7" s="3" t="n">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="P7" s="4" t="n">
-        <v>44.07692307692308</v>
+        <v>42.84615384615385</v>
       </c>
       <c r="Q7" s="3" t="n">
         <v>40</v>
@@ -950,7 +998,7 @@
         <v>22</v>
       </c>
       <c r="C8" s="3" t="n">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D8" s="3" t="n">
         <v>42</v>
@@ -980,16 +1028,16 @@
         <v>42</v>
       </c>
       <c r="M8" s="3" t="n">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="N8" s="3" t="n">
-        <v>43.5</v>
+        <v>35.5</v>
       </c>
       <c r="O8" s="3" t="n">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="P8" s="4" t="n">
-        <v>42.30769230769231</v>
+        <v>38.61538461538461</v>
       </c>
       <c r="Q8" s="3" t="n">
         <v>40</v>
@@ -1003,7 +1051,7 @@
         <v>23</v>
       </c>
       <c r="C9" s="3" t="n">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D9" s="3" t="n">
         <v>49.5</v>
@@ -1030,19 +1078,19 @@
         <v>50</v>
       </c>
       <c r="L9" s="3" t="n">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="M9" s="3" t="n">
         <v>40</v>
       </c>
       <c r="N9" s="3" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="O9" s="3" t="n">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="P9" s="4" t="n">
-        <v>43.46153846153846</v>
+        <v>39</v>
       </c>
       <c r="Q9" s="3" t="n">
         <v>40</v>
@@ -1056,10 +1104,10 @@
         <v>24</v>
       </c>
       <c r="C10" s="3" t="n">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="D10" s="3" t="n">
-        <v>43.5</v>
+        <v>40.5</v>
       </c>
       <c r="E10" s="3" t="n">
         <v>46</v>
@@ -1071,7 +1119,7 @@
         <v>45.5</v>
       </c>
       <c r="H10" s="3" t="n">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="I10" s="3" t="n">
         <v>57</v>
@@ -1089,13 +1137,13 @@
         <v>53.5</v>
       </c>
       <c r="N10" s="3" t="n">
-        <v>44.5</v>
+        <v>36.5</v>
       </c>
       <c r="O10" s="3" t="n">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="P10" s="4" t="n">
-        <v>46.88461538461539</v>
+        <v>41.11538461538461</v>
       </c>
       <c r="Q10" s="3" t="n">
         <v>40</v>
@@ -1109,7 +1157,7 @@
         <v>25</v>
       </c>
       <c r="C11" s="3" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="D11" s="3" t="n">
         <v>36</v>
@@ -1121,7 +1169,7 @@
         <v>40</v>
       </c>
       <c r="G11" s="3" t="n">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H11" s="3" t="n">
         <v>40</v>
@@ -1148,7 +1196,7 @@
         <v>40</v>
       </c>
       <c r="P11" s="4" t="n">
-        <v>39.69230769230769</v>
+        <v>36.30769230769231</v>
       </c>
       <c r="Q11" s="3" t="n">
         <v>40</v>
@@ -1215,7 +1263,7 @@
         <v>27</v>
       </c>
       <c r="C13" s="3" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="D13" s="3" t="n">
         <v>61</v>
@@ -1254,7 +1302,7 @@
         <v>40</v>
       </c>
       <c r="P13" s="4" t="n">
-        <v>46.46153846153846</v>
+        <v>43.38461538461539</v>
       </c>
       <c r="Q13" s="3" t="n">
         <v>40</v>
@@ -1301,13 +1349,13 @@
         <v>40</v>
       </c>
       <c r="N14" s="3" t="n">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="O14" s="3" t="n">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="P14" s="4" t="n">
-        <v>12.30769230769231</v>
+        <v>11.07692307692308</v>
       </c>
       <c r="Q14" s="3" t="n">
         <v>40</v>
@@ -1321,7 +1369,7 @@
         <v>29</v>
       </c>
       <c r="C15" s="3" t="n">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="D15" s="3" t="n">
         <v>44</v>
@@ -1348,19 +1396,19 @@
         <v>48</v>
       </c>
       <c r="L15" s="3" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="M15" s="3" t="n">
         <v>44</v>
       </c>
       <c r="N15" s="3" t="n">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="O15" s="3" t="n">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="P15" s="4" t="n">
-        <v>44.38461538461539</v>
+        <v>38.23076923076923</v>
       </c>
       <c r="Q15" s="3" t="n">
         <v>40</v>
@@ -1407,13 +1455,13 @@
         <v>50</v>
       </c>
       <c r="N16" s="3" t="n">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="O16" s="3" t="n">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="P16" s="4" t="n">
-        <v>40.84615384615385</v>
+        <v>37.15384615384615</v>
       </c>
       <c r="Q16" s="3" t="n">
         <v>40</v>
@@ -1427,7 +1475,7 @@
         <v>31</v>
       </c>
       <c r="C17" s="3" t="n">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D17" s="3" t="n">
         <v>42.5</v>
@@ -1448,7 +1496,7 @@
         <v>44.5</v>
       </c>
       <c r="J17" s="3" t="n">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="K17" s="3" t="n">
         <v>46.5</v>
@@ -1457,16 +1505,16 @@
         <v>46</v>
       </c>
       <c r="M17" s="3" t="n">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="N17" s="3" t="n">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="O17" s="3" t="n">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="P17" s="4" t="n">
-        <v>45.80769230769231</v>
+        <v>41.73076923076923</v>
       </c>
       <c r="Q17" s="3" t="n">
         <v>37.5</v>
@@ -1489,10 +1537,10 @@
         <v>45</v>
       </c>
       <c r="F18" s="3" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="G18" s="3" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="H18" s="3" t="n">
         <v>43.5</v>
@@ -1513,13 +1561,13 @@
         <v>42</v>
       </c>
       <c r="N18" s="3" t="n">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="O18" s="3" t="n">
         <v>40.5</v>
       </c>
       <c r="P18" s="4" t="n">
-        <v>42.07692307692308</v>
+        <v>35.30769230769231</v>
       </c>
       <c r="Q18" s="3" t="n">
         <v>40</v>
@@ -1545,7 +1593,7 @@
         <v>38</v>
       </c>
       <c r="G19" s="6" t="n">
-        <v>37.5</v>
+        <v>30</v>
       </c>
       <c r="H19" s="6" t="n">
         <v>43.5</v>
@@ -1560,19 +1608,19 @@
         <v>51</v>
       </c>
       <c r="L19" s="6" t="n">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="M19" s="6" t="n">
         <v>46</v>
       </c>
       <c r="N19" s="6" t="n">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="O19" s="6" t="n">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="P19" s="7" t="n">
-        <v>41.26923076923077</v>
+        <v>38.23076923076923</v>
       </c>
       <c r="Q19" s="6" t="n">
         <v>37.5</v>
@@ -1645,16 +1693,16 @@
         <v>52.5</v>
       </c>
       <c r="F22" s="3" t="n">
-        <v>0</v>
+        <v>37.5</v>
       </c>
       <c r="G22" s="3" t="n">
-        <v>0</v>
+        <v>37.5</v>
       </c>
       <c r="H22" s="3" t="n">
-        <v>0</v>
+        <v>37.5</v>
       </c>
       <c r="I22" s="3" t="n">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="J22" s="3" t="n">
         <v>59</v>
@@ -1666,16 +1714,16 @@
         <v>52</v>
       </c>
       <c r="M22" s="3" t="n">
-        <v>35.5</v>
+        <v>38.5</v>
       </c>
       <c r="N22" s="3" t="n">
-        <v>34.5</v>
+        <v>42.5</v>
       </c>
       <c r="O22" s="3" t="n">
         <v>48.5</v>
       </c>
       <c r="P22" s="4" t="n">
-        <v>39.03846153846154</v>
+        <v>48.76923076923077</v>
       </c>
       <c r="Q22" s="5" t="n">
         <v>37.5</v>
@@ -1695,7 +1743,7 @@
         <v>60.5</v>
       </c>
       <c r="F23" s="3" t="n">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="G23" s="3" t="n">
         <v>40</v>
@@ -1710,7 +1758,7 @@
         <v>50.5</v>
       </c>
       <c r="K23" s="3" t="n">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="L23" s="3" t="n">
         <v>47</v>
@@ -1719,13 +1767,13 @@
         <v>66</v>
       </c>
       <c r="N23" s="3" t="n">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="O23" s="3" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="P23" s="4" t="n">
-        <v>46.42307692307692</v>
+        <v>49.26923076923077</v>
       </c>
       <c r="Q23" s="5" t="n">
         <v>37.5</v>
@@ -1745,7 +1793,7 @@
         <v>37.5</v>
       </c>
       <c r="F24" s="3" t="n">
-        <v>15</v>
+        <v>37.5</v>
       </c>
       <c r="G24" s="3" t="n">
         <v>37.5</v>
@@ -1769,13 +1817,13 @@
         <v>38</v>
       </c>
       <c r="N24" s="3" t="n">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="O24" s="3" t="n">
-        <v>21.5</v>
+        <v>37.5</v>
       </c>
       <c r="P24" s="4" t="n">
-        <v>34.42307692307692</v>
+        <v>38</v>
       </c>
       <c r="Q24" s="5" t="n">
         <v>37.5</v>
@@ -1819,13 +1867,13 @@
         <v>42</v>
       </c>
       <c r="N25" s="3" t="n">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="O25" s="3" t="n">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="P25" s="4" t="n">
-        <v>43.57692307692308</v>
+        <v>44.80769230769231</v>
       </c>
       <c r="Q25" s="5" t="n">
         <v>37.5</v>
@@ -1869,13 +1917,13 @@
         <v>42</v>
       </c>
       <c r="N26" s="3" t="n">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="O26" s="3" t="n">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="P26" s="4" t="n">
-        <v>42.84615384615385</v>
+        <v>44.07692307692308</v>
       </c>
       <c r="Q26" s="5" t="n">
         <v>40</v>
@@ -1886,7 +1934,7 @@
         <v>22</v>
       </c>
       <c r="C27" s="3" t="n">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="D27" s="3" t="n">
         <v>42</v>
@@ -1916,16 +1964,16 @@
         <v>42</v>
       </c>
       <c r="M27" s="3" t="n">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="N27" s="3" t="n">
-        <v>35.5</v>
+        <v>43.5</v>
       </c>
       <c r="O27" s="3" t="n">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="P27" s="4" t="n">
-        <v>38.61538461538461</v>
+        <v>42.30769230769231</v>
       </c>
       <c r="Q27" s="5" t="n">
         <v>40</v>
@@ -1936,7 +1984,7 @@
         <v>23</v>
       </c>
       <c r="C28" s="3" t="n">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="D28" s="3" t="n">
         <v>49.5</v>
@@ -1963,19 +2011,19 @@
         <v>50</v>
       </c>
       <c r="L28" s="3" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="M28" s="3" t="n">
         <v>40</v>
       </c>
       <c r="N28" s="3" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="O28" s="3" t="n">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="P28" s="4" t="n">
-        <v>39</v>
+        <v>43.46153846153846</v>
       </c>
       <c r="Q28" s="5" t="n">
         <v>40</v>
@@ -1986,10 +2034,10 @@
         <v>24</v>
       </c>
       <c r="C29" s="3" t="n">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="D29" s="3" t="n">
-        <v>40.5</v>
+        <v>43.5</v>
       </c>
       <c r="E29" s="3" t="n">
         <v>46</v>
@@ -2001,7 +2049,7 @@
         <v>45.5</v>
       </c>
       <c r="H29" s="3" t="n">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="I29" s="3" t="n">
         <v>57</v>
@@ -2019,13 +2067,13 @@
         <v>53.5</v>
       </c>
       <c r="N29" s="3" t="n">
-        <v>36.5</v>
+        <v>44.5</v>
       </c>
       <c r="O29" s="3" t="n">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="P29" s="4" t="n">
-        <v>41.11538461538461</v>
+        <v>46.88461538461539</v>
       </c>
       <c r="Q29" s="5" t="n">
         <v>40</v>
@@ -2036,7 +2084,7 @@
         <v>25</v>
       </c>
       <c r="C30" s="3" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="D30" s="3" t="n">
         <v>36</v>
@@ -2048,7 +2096,7 @@
         <v>40</v>
       </c>
       <c r="G30" s="3" t="n">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="H30" s="3" t="n">
         <v>40</v>
@@ -2075,7 +2123,7 @@
         <v>40</v>
       </c>
       <c r="P30" s="4" t="n">
-        <v>36.30769230769231</v>
+        <v>39.69230769230769</v>
       </c>
       <c r="Q30" s="5" t="n">
         <v>40</v>
@@ -2136,7 +2184,7 @@
         <v>27</v>
       </c>
       <c r="C32" s="3" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="D32" s="3" t="n">
         <v>61</v>
@@ -2175,7 +2223,7 @@
         <v>40</v>
       </c>
       <c r="P32" s="4" t="n">
-        <v>43.38461538461539</v>
+        <v>46.46153846153846</v>
       </c>
       <c r="Q32" s="5" t="n">
         <v>40</v>
@@ -2219,13 +2267,13 @@
         <v>40</v>
       </c>
       <c r="N33" s="3" t="n">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="O33" s="3" t="n">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="P33" s="4" t="n">
-        <v>11.07692307692308</v>
+        <v>12.30769230769231</v>
       </c>
       <c r="Q33" s="5" t="n">
         <v>40</v>
@@ -2236,7 +2284,7 @@
         <v>29</v>
       </c>
       <c r="C34" s="3" t="n">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="D34" s="3" t="n">
         <v>44</v>
@@ -2263,19 +2311,19 @@
         <v>48</v>
       </c>
       <c r="L34" s="3" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="M34" s="3" t="n">
         <v>44</v>
       </c>
       <c r="N34" s="3" t="n">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="O34" s="3" t="n">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="P34" s="4" t="n">
-        <v>38.23076923076923</v>
+        <v>44.38461538461539</v>
       </c>
       <c r="Q34" s="5" t="n">
         <v>40</v>
@@ -2319,13 +2367,13 @@
         <v>50</v>
       </c>
       <c r="N35" s="3" t="n">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="O35" s="3" t="n">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="P35" s="4" t="n">
-        <v>37.15384615384615</v>
+        <v>40.84615384615385</v>
       </c>
       <c r="Q35" s="5" t="n">
         <v>40</v>
@@ -2336,7 +2384,7 @@
         <v>31</v>
       </c>
       <c r="C36" s="3" t="n">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="D36" s="3" t="n">
         <v>42.5</v>
@@ -2357,7 +2405,7 @@
         <v>44.5</v>
       </c>
       <c r="J36" s="3" t="n">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="K36" s="3" t="n">
         <v>46.5</v>
@@ -2366,16 +2414,16 @@
         <v>46</v>
       </c>
       <c r="M36" s="3" t="n">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="N36" s="3" t="n">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="O36" s="3" t="n">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="P36" s="4" t="n">
-        <v>41.73076923076923</v>
+        <v>45.80769230769231</v>
       </c>
       <c r="Q36" s="5" t="n">
         <v>37.5</v>
@@ -2395,10 +2443,10 @@
         <v>45</v>
       </c>
       <c r="F37" s="3" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="G37" s="3" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="H37" s="3" t="n">
         <v>43.5</v>
@@ -2419,13 +2467,13 @@
         <v>42</v>
       </c>
       <c r="N37" s="3" t="n">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="O37" s="3" t="n">
         <v>40.5</v>
       </c>
       <c r="P37" s="4" t="n">
-        <v>35.30769230769231</v>
+        <v>42.07692307692308</v>
       </c>
       <c r="Q37" s="5" t="n">
         <v>40</v>
@@ -2448,7 +2496,7 @@
         <v>38</v>
       </c>
       <c r="G38" s="6" t="n">
-        <v>30</v>
+        <v>37.5</v>
       </c>
       <c r="H38" s="6" t="n">
         <v>43.5</v>
@@ -2463,22 +2511,1009 @@
         <v>51</v>
       </c>
       <c r="L38" s="6" t="n">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="M38" s="6" t="n">
         <v>46</v>
       </c>
       <c r="N38" s="6" t="n">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="O38" s="6" t="n">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="P38" s="7" t="n">
-        <v>38.23076923076923</v>
+        <v>41.26923076923077</v>
       </c>
       <c r="Q38" s="8" t="n">
         <v>37.5</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="40" r="40" spans="1:18">
+      <c r="B40" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O40" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P40" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="41" spans="1:18">
+      <c r="B41" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" s="3" t="n">
+        <v>390.5</v>
+      </c>
+      <c r="D41" s="3" t="n">
+        <v>403</v>
+      </c>
+      <c r="E41" s="3" t="n">
+        <v>417.5</v>
+      </c>
+      <c r="F41" s="3" t="n">
+        <v>402</v>
+      </c>
+      <c r="G41" s="3" t="n">
+        <v>380.5</v>
+      </c>
+      <c r="H41" s="3" t="n">
+        <v>390</v>
+      </c>
+      <c r="I41" s="3" t="n">
+        <v>447.5</v>
+      </c>
+      <c r="J41" s="3" t="n">
+        <v>418.5</v>
+      </c>
+      <c r="K41" s="3" t="n">
+        <v>410</v>
+      </c>
+      <c r="L41" s="3" t="n">
+        <v>412</v>
+      </c>
+      <c r="M41" s="3" t="n">
+        <v>404</v>
+      </c>
+      <c r="N41" s="3" t="n">
+        <v>397</v>
+      </c>
+      <c r="O41" s="3" t="n">
+        <v>372.5</v>
+      </c>
+      <c r="P41" s="9" t="n">
+        <v>403.4615384615385</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="42" spans="1:18">
+      <c r="B42" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" s="6" t="n">
+        <v>290.5</v>
+      </c>
+      <c r="D42" s="6" t="n">
+        <v>305.5</v>
+      </c>
+      <c r="E42" s="6" t="n">
+        <v>295</v>
+      </c>
+      <c r="F42" s="6" t="n">
+        <v>297</v>
+      </c>
+      <c r="G42" s="6" t="n">
+        <v>309</v>
+      </c>
+      <c r="H42" s="6" t="n">
+        <v>309</v>
+      </c>
+      <c r="I42" s="6" t="n">
+        <v>305.5</v>
+      </c>
+      <c r="J42" s="6" t="n">
+        <v>294.5</v>
+      </c>
+      <c r="K42" s="6" t="n">
+        <v>305</v>
+      </c>
+      <c r="L42" s="6" t="n">
+        <v>348</v>
+      </c>
+      <c r="M42" s="6" t="n">
+        <v>359.5</v>
+      </c>
+      <c r="N42" s="6" t="n">
+        <v>336</v>
+      </c>
+      <c r="O42" s="6" t="n">
+        <v>328.5</v>
+      </c>
+      <c r="P42" s="10" t="n">
+        <v>314.0769230769231</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="40" r="44" spans="1:18">
+      <c r="B44" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N44" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O44" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P44" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="45" spans="1:18">
+      <c r="B45" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C45" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="D45" s="3" t="n">
+        <v>24.5</v>
+      </c>
+      <c r="E45" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="F45" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I45" s="3" t="n">
+        <v>28.5</v>
+      </c>
+      <c r="J45" s="3" t="n">
+        <v>21.5</v>
+      </c>
+      <c r="K45" s="3" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L45" s="3" t="n">
+        <v>14.5</v>
+      </c>
+      <c r="M45" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N45" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="O45" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="P45" s="9" t="n">
+        <v>11.26923076923077</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="46" spans="1:18">
+      <c r="B46" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46" s="3" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D46" s="3" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="E46" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="F46" s="3" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="G46" s="3" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H46" s="3" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="I46" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="J46" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="K46" s="3" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="L46" s="3" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="M46" s="3" t="n">
+        <v>28.5</v>
+      </c>
+      <c r="N46" s="3" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="O46" s="3" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="P46" s="9" t="n">
+        <v>11.76923076923077</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="47" spans="1:18">
+      <c r="B47" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C47" s="3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D47" s="3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E47" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F47" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H47" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I47" s="3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J47" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K47" s="3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L47" s="3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M47" s="3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="N47" s="3" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="O47" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P47" s="9" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="48" spans="1:18">
+      <c r="B48" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C48" s="3" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D48" s="3" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="E48" s="3" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F48" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="G48" s="3" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="H48" s="3" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="I48" s="3" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="J48" s="3" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="K48" s="3" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="L48" s="3" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="M48" s="3" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="N48" s="3" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="O48" s="3" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="P48" s="9" t="n">
+        <v>7.307692307692307</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="49" spans="1:18">
+      <c r="B49" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C49" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D49" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E49" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="F49" s="3" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G49" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="H49" s="3" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="I49" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J49" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="K49" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="L49" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="M49" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="N49" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="O49" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="P49" s="9" t="n">
+        <v>4.076923076923077</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="50" spans="1:18">
+      <c r="B50" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C50" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D50" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E50" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F50" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H50" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="I50" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="J50" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K50" s="3" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="L50" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="M50" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="N50" s="3" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="O50" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="P50" s="9" t="n">
+        <v>2.307692307692307</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="51" spans="1:18">
+      <c r="B51" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C51" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D51" s="3" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="E51" s="3" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F51" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G51" s="3" t="n">
+        <v>-2</v>
+      </c>
+      <c r="H51" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="I51" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="J51" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="K51" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="L51" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="M51" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N51" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O51" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P51" s="9" t="n">
+        <v>3.461538461538462</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="52" spans="1:18">
+      <c r="B52" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C52" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D52" s="3" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="E52" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="F52" s="3" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="G52" s="3" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="H52" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="I52" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="J52" s="3" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="K52" s="3" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="L52" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="M52" s="3" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="N52" s="3" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="O52" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="P52" s="9" t="n">
+        <v>6.884615384615385</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="53" spans="1:18">
+      <c r="B53" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C53" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D53" s="3" t="n">
+        <v>-4</v>
+      </c>
+      <c r="E53" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F53" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G53" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H53" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I53" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J53" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K53" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L53" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M53" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N53" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O53" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P53" s="9" t="n">
+        <v>-0.3076923076923077</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="54" spans="1:18">
+      <c r="B54" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C54" s="3" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="D54" s="3" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="E54" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="F54" s="3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G54" s="3" t="n">
+        <v>16.5</v>
+      </c>
+      <c r="H54" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I54" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="J54" s="3" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="K54" s="3" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="L54" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M54" s="3" t="n">
+        <v>17.5</v>
+      </c>
+      <c r="N54" s="3" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="O54" s="3" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="P54" s="9" t="n">
+        <v>7.115384615384615</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="55" spans="1:18">
+      <c r="B55" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C55" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D55" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="E55" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F55" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="G55" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H55" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="I55" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J55" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="K55" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="L55" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="M55" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N55" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O55" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P55" s="9" t="n">
+        <v>6.461538461538462</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="56" spans="1:18">
+      <c r="B56" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C56" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D56" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E56" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F56" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G56" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H56" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I56" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J56" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K56" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L56" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M56" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N56" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O56" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P56" s="9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="57" spans="1:18">
+      <c r="B57" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C57" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D57" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E57" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F57" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G57" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="H57" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="I57" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J57" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="K57" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L57" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M57" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="N57" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="O57" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P57" s="9" t="n">
+        <v>4.384615384615385</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="58" spans="1:18">
+      <c r="B58" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C58" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D58" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E58" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F58" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G58" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H58" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I58" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J58" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K58" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L58" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M58" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="N58" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O58" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P58" s="9" t="n">
+        <v>0.8461538461538461</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="59" spans="1:18">
+      <c r="B59" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C59" s="3" t="n">
+        <v>16.5</v>
+      </c>
+      <c r="D59" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="E59" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="F59" s="3" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="G59" s="3" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="H59" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="I59" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="J59" s="3" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="K59" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="L59" s="3" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="M59" s="3" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="N59" s="3" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="O59" s="3" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="P59" s="9" t="n">
+        <v>8.307692307692308</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="60" spans="1:18">
+      <c r="B60" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C60" s="3" t="n">
+        <v>-7</v>
+      </c>
+      <c r="D60" s="3" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="E60" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="F60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H60" s="3" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="I60" s="3" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="J60" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="K60" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="L60" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="M60" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="N60" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="O60" s="3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="P60" s="9" t="n">
+        <v>2.076923076923077</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="61" spans="1:18">
+      <c r="B61" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C61" s="6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D61" s="6" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E61" s="6" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F61" s="6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G61" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H61" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="I61" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="J61" s="6" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="K61" s="6" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="L61" s="6" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="M61" s="6" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="N61" s="6" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="O61" s="6" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="P61" s="10" t="n">
+        <v>3.769230769230769</v>
       </c>
     </row>
   </sheetData>

</xml_diff>